<commit_message>
add more tables and figures for presentation
</commit_message>
<xml_diff>
--- a/figures/time-invariant-figure.xlsx
+++ b/figures/time-invariant-figure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\covid-rent-study\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32CE886E-03D0-4F06-81EB-A90D103AF7E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CCF307-7EFD-4C12-AF0F-88405BD1985A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E5BC6F13-B9AC-42E3-AC7A-DB63DEDD7F54}"/>
+    <workbookView xWindow="1704" yWindow="0" windowWidth="20364" windowHeight="12492" xr2:uid="{E5BC6F13-B9AC-42E3-AC7A-DB63DEDD7F54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -371,22 +371,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18F303AD-61D9-4DC4-980C-4EECACED43FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB2D631C-DC14-4622-92D6-C0F8F0FB0E31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -409,7 +409,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6629400" y="182880"/>
+          <a:off x="6644640" y="45720"/>
           <a:ext cx="5417820" cy="5722620"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D1FCEF-71EA-4A48-9FDA-20E837309E13}">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>